<commit_message>
fix corrupted excel file
</commit_message>
<xml_diff>
--- a/TestExcel.xlsx
+++ b/TestExcel.xlsx
@@ -7,6 +7,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Manipulated_Data" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Manipulated_Data2" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -448,4 +450,132 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>selamlar</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>selamlar</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>merhaba</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>merhaba</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>deneme</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>deneme</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>selamlar</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>selamlar</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>merhaba</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>merhaba</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>deneme</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>deneme</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
load plugins dynamically from workflow
</commit_message>
<xml_diff>
--- a/TestExcel.xlsx
+++ b/TestExcel.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="37035" yWindow="2685" windowWidth="14925" windowHeight="9960" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5832" yWindow="2004" windowWidth="14928" windowHeight="9960" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Manipulated_Data2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 

</xml_diff>

<commit_message>
return boolean if plugin loaded correctly
</commit_message>
<xml_diff>
--- a/TestExcel.xlsx
+++ b/TestExcel.xlsx
@@ -476,7 +476,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>selamlar_manipulated plugin</t>
+          <t>selamlar_manipulated_plugin2</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>merhaba_manipulated plugin</t>
+          <t>merhaba_manipulated_plugin2</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>deneme_manipulated plugin</t>
+          <t>deneme_manipulated_plugin2</t>
         </is>
       </c>
     </row>

</xml_diff>